<commit_message>
Better integration between scripts
</commit_message>
<xml_diff>
--- a/Sample_sheet_test.xlsx
+++ b/Sample_sheet_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NormRcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TURAKU~1\DOCUME~1\MobaXterm\slash\RemoteFiles\132350_3_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907C15E2-B352-4497-AD42-001EC2D5517B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3CEAB8-0160-478D-9D3D-112C4AE0CC93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{21331885-AE57-439C-8433-44AC06AA1335}"/>
+    <workbookView xWindow="20300" yWindow="1100" windowWidth="28800" windowHeight="15460" xr2:uid="{21331885-AE57-439C-8433-44AC06AA1335}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="210">
   <si>
     <t>order</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>idat/204095630005_R01C01</t>
+  </si>
+  <si>
+    <t>Frozen</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A33B3D-C194-49FC-B65A-CC04E1C02A0A}">
   <dimension ref="A1:DQ1375"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1483,7 +1486,7 @@
         <v>125</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="AG2" s="1" t="s">
         <v>127</v>
@@ -1607,7 +1610,7 @@
         <v>140</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="AG3" s="1" t="s">
         <v>127</v>
@@ -1750,7 +1753,7 @@
         <v>140</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="AG4" s="1" t="s">
         <v>127</v>
@@ -1877,7 +1880,7 @@
         <v>140</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>126</v>
+        <v>209</v>
       </c>
       <c r="AG5" s="1" t="s">
         <v>127</v>

</xml_diff>